<commit_message>
Updated with 2019 Import Export Data
</commit_message>
<xml_diff>
--- a/raw-data/Trade Turnover.xlsx
+++ b/raw-data/Trade Turnover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\southcaucasus\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D60EEA-33D4-4B8A-B4AE-60B039BB1613}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76CE1A5-4F69-42EB-B92B-1BBCF6116481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0B522DDE-64AF-444D-9BCA-C1E2C8819BBC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="6">
   <si>
     <t>Azerbaijan</t>
   </si>
@@ -179,7 +179,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -200,6 +200,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,20 +520,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50E2B15-C8F4-471D-90D8-70A3A96D22B0}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.453125" customWidth="1"/>
     <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -541,7 +546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -552,7 +557,7 @@
         <v>273049.7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -563,7 +568,7 @@
         <v>228883.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -574,7 +579,7 @@
         <v>288915.90000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -585,7 +590,7 @@
         <v>977802.4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -596,7 +601,7 @@
         <v>615034.30000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -607,7 +612,7 @@
         <v>926469.2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -618,7 +623,7 @@
         <v>667261.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -629,7 +634,7 @@
         <v>815625</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -640,7 +645,7 @@
         <v>654972.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -651,7 +656,7 @@
         <v>760945.4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -662,7 +667,7 @@
         <v>565111.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -673,7 +678,7 @@
         <v>1085832.7999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -684,7 +689,7 @@
         <v>1298342.3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -694,314 +699,355 @@
       <c r="C15" s="3">
         <v>1310247</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B16">
+        <v>2019</v>
+      </c>
+      <c r="C16" s="8">
+        <v>2184313.08</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
         <v>2005</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C17" s="7">
         <v>35379.760000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
         <v>2006</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C18" s="7">
         <v>109998.99</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
         <v>2007</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C19" s="7">
         <v>200218.18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
         <v>2008</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C20" s="7">
         <v>378044.94</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
         <v>2009</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C21" s="7">
         <v>302683.75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
         <v>2010</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C22" s="7">
         <v>432943.45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
         <v>2011</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C23" s="7">
         <v>418801.95</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
         <v>2012</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C24" s="7">
         <v>428066.93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
         <v>2013</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C25" s="7">
         <v>452329.42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
         <v>2014</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C26" s="7">
         <v>585372.87</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
         <v>2015</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C27" s="7">
         <v>480671.77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
         <v>2016</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C28" s="7">
         <v>463127.64</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
         <v>2017</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C29" s="7">
         <v>584344.73</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
         <v>2018</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C30" s="7">
         <v>768339.87</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30">
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>2019</v>
+      </c>
+      <c r="C31" s="7">
+        <v>941705.76</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
         <v>2005</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C32" s="7">
         <v>51935.199999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33">
         <v>2006</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C33" s="7">
         <v>113554.46</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
         <v>2007</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C34" s="7">
         <v>214619.39</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
         <v>2008</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C35" s="7">
         <v>306455.90999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
         <v>2009</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C36" s="7">
         <v>180536.84</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37">
         <v>2010</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C37" s="7">
         <v>362210.43</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
         <v>2011</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C38" s="7">
         <v>556671.12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
         <v>2012</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C39" s="7">
         <v>640091.4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
         <v>2013</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C40" s="7">
         <v>646206.15</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
         <v>2014</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C41" s="7">
         <v>823860.88</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
         <v>2015</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C42" s="7">
         <v>713157.46</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
         <v>2016</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C43" s="7">
         <v>717069.46</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44">
         <v>2017</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C44" s="7">
         <v>934647.57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45">
         <v>2018</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C45" s="7">
         <v>1031922.73</v>
       </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>2019</v>
+      </c>
+      <c r="C46" s="7">
+        <v>1081719.3500000001</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>